<commit_message>
Updated a couple of files
Changed the location of images, an created a file for Tomasz.
</commit_message>
<xml_diff>
--- a/Documenten/Urenlijst.xlsx
+++ b/Documenten/Urenlijst.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Tomasz" sheetId="4" r:id="rId1"/>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,8 +625,12 @@
       <c r="E3" s="6">
         <v>0.5</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="F3" s="6">
+        <v>4</v>
+      </c>
+      <c r="G3" s="6">
+        <v>4</v>
+      </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
     </row>
@@ -725,7 +729,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>4.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1300,7 +1304,7 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,8 +1355,12 @@
       <c r="E3" s="6">
         <v>4</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="F3" s="6">
+        <v>4</v>
+      </c>
+      <c r="G3" s="6">
+        <v>4</v>
+      </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
     </row>
@@ -1451,7 +1459,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2026,7 +2034,7 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2077,8 +2085,12 @@
       <c r="E3" s="6">
         <v>4</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="F3" s="6">
+        <v>4</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
     </row>
@@ -2177,7 +2189,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2751,8 +2763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2803,8 +2815,12 @@
       <c r="E3" s="6">
         <v>4</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="F3" s="6">
+        <v>4</v>
+      </c>
+      <c r="G3" s="6">
+        <v>4</v>
+      </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
     </row>
@@ -2903,7 +2919,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
toevoegen van de techniche test en bijwerken van wat ik gister aangepast had
</commit_message>
<xml_diff>
--- a/Documenten/Urenlijst.xlsx
+++ b/Documenten/Urenlijst.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tomasz" sheetId="4" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Remco" sheetId="2" r:id="rId3"/>
     <sheet name="Max" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +638,9 @@
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="7">
+        <v>4</v>
+      </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -729,7 +731,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>12.5</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1304,7 +1306,7 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,7 +1370,9 @@
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="7">
+        <v>4</v>
+      </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -1459,7 +1463,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2034,7 +2038,7 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2098,7 +2102,9 @@
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="7">
+        <v>4</v>
+      </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -2189,7 +2195,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2763,8 +2769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2828,7 +2834,9 @@
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="7">
+        <v>4</v>
+      </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -2919,7 +2927,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated almost all files
I changed the mistakes in the documents.
</commit_message>
<xml_diff>
--- a/Documenten/Urenlijst.xlsx
+++ b/Documenten/Urenlijst.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tomasz" sheetId="4" r:id="rId1"/>
@@ -573,7 +573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
@@ -1307,8 +1307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,7 +1376,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -1467,7 +1467,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Logboek en Urenlijst aangepast.
</commit_message>
<xml_diff>
--- a/Documenten/Urenlijst.xlsx
+++ b/Documenten/Urenlijst.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Tomasz" sheetId="4" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Remco" sheetId="2" r:id="rId3"/>
     <sheet name="Max" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,13 +617,13 @@
         <v>9</v>
       </c>
       <c r="C3" s="5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D3" s="6">
         <v>4</v>
       </c>
       <c r="E3" s="6">
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="F3" s="6">
         <v>4</v>
@@ -631,8 +631,12 @@
       <c r="G3" s="6">
         <v>4</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="H3" s="6">
+        <v>2</v>
+      </c>
+      <c r="I3" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -653,7 +657,9 @@
       <c r="G4" s="8">
         <v>0</v>
       </c>
-      <c r="H4" s="8"/>
+      <c r="H4" s="8">
+        <v>1</v>
+      </c>
       <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -675,8 +681,12 @@
       <c r="G5" s="11">
         <v>4</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
+      <c r="H5" s="11">
+        <v>2</v>
+      </c>
+      <c r="I5" s="11">
+        <v>3</v>
+      </c>
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -684,7 +694,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6" s="11">
         <v>0</v>
@@ -696,7 +706,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="11">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="7"/>
@@ -759,7 +769,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>44.5</v>
+        <v>64.5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1332,7 +1342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated "Urenlijst en logboek"
</commit_message>
<xml_diff>
--- a/Documenten/Urenlijst.xlsx
+++ b/Documenten/Urenlijst.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
-  <workbookPr filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tomasz" sheetId="4" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Remco" sheetId="2" r:id="rId3"/>
     <sheet name="Max" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +660,9 @@
       <c r="H4" s="8">
         <v>1</v>
       </c>
-      <c r="I4" s="8"/>
+      <c r="I4" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
@@ -708,8 +710,12 @@
       <c r="G6" s="11">
         <v>0.5</v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="7"/>
+      <c r="H6" s="11">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0</v>
+      </c>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
     </row>
@@ -717,7 +723,9 @@
       <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="5">
+        <v>4</v>
+      </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -769,7 +777,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>64.5</v>
+        <v>68.5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1342,8 +1350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1480,7 +1488,9 @@
       <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="5">
+        <v>4</v>
+      </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -1532,7 +1542,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>76.5</v>
+        <v>80.5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2107,7 +2117,7 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2240,7 +2250,9 @@
       <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="5">
+        <v>4</v>
+      </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -2292,7 +2304,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>57.2</v>
+        <v>61.2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2867,7 +2879,7 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20:G20"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3000,7 +3012,9 @@
       <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="5">
+        <v>4</v>
+      </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -3052,7 +3066,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated "Logboek en urenlijst"
</commit_message>
<xml_diff>
--- a/Documenten/Urenlijst.xlsx
+++ b/Documenten/Urenlijst.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tomasz" sheetId="4" r:id="rId1"/>
@@ -574,7 +574,7 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,7 +726,9 @@
       <c r="C7" s="5">
         <v>4</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="6">
+        <v>4</v>
+      </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -777,7 +779,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>68.5</v>
+        <v>72.5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1350,8 +1352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1491,7 +1493,9 @@
       <c r="C7" s="5">
         <v>4</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="6">
+        <v>4</v>
+      </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -1542,7 +1546,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>80.5</v>
+        <v>84.5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2117,7 +2121,7 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2253,7 +2257,9 @@
       <c r="C7" s="5">
         <v>4</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="6">
+        <v>4</v>
+      </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -2304,7 +2310,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>61.2</v>
+        <v>65.2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2878,8 +2884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3015,7 +3021,9 @@
       <c r="C7" s="5">
         <v>4</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="6">
+        <v>4</v>
+      </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -3066,7 +3074,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated urenlijst en logboek
</commit_message>
<xml_diff>
--- a/Documenten/Urenlijst.xlsx
+++ b/Documenten/Urenlijst.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -12,7 +12,7 @@
     <sheet name="Remco" sheetId="2" r:id="rId3"/>
     <sheet name="Max" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -574,7 +574,7 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,13 +727,13 @@
         <v>4</v>
       </c>
       <c r="D7" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E7" s="6">
         <v>4</v>
       </c>
       <c r="F7" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G7" s="6">
         <v>4</v>
@@ -785,7 +785,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>84.5</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated "Urenlijst and Logboek"
</commit_message>
<xml_diff>
--- a/Documenten/Urenlijst.xlsx
+++ b/Documenten/Urenlijst.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Tomasz" sheetId="4" r:id="rId1"/>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2914,8 +2914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3061,10 +3061,12 @@
         <v>4</v>
       </c>
       <c r="G7" s="6">
-        <v>4</v>
+        <v>4.25</v>
       </c>
       <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="I7" s="6">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -3114,7 +3116,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>101</v>
+        <v>104.75</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated logboek en urenlijst
</commit_message>
<xml_diff>
--- a/Documenten/Urenlijst.xlsx
+++ b/Documenten/Urenlijst.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Tomasz" sheetId="4" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Remco" sheetId="2" r:id="rId3"/>
     <sheet name="Max" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +696,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D6" s="11">
         <v>0</v>
@@ -746,12 +746,14 @@
         <v>15</v>
       </c>
       <c r="C8" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D8" s="8">
         <v>4</v>
       </c>
-      <c r="E8" s="8"/>
+      <c r="E8" s="8">
+        <v>4</v>
+      </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
@@ -789,7 +791,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>91.5</v>
+        <v>100.5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1362,7 +1364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated urenlijst & pve
updated urenlijst & pve
</commit_message>
<xml_diff>
--- a/Documenten/Urenlijst.xlsx
+++ b/Documenten/Urenlijst.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Tomasz" sheetId="4" r:id="rId1"/>
@@ -607,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,8 +807,12 @@
       <c r="D9" s="11">
         <v>4</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="E9" s="11">
+        <v>4</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0</v>
+      </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
@@ -833,7 +837,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>119.5</v>
+        <v>123.5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1407,7 +1411,7 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I21:I22"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1594,8 +1598,12 @@
       <c r="D9" s="11">
         <v>4</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="E9" s="11">
+        <v>4</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0</v>
+      </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
@@ -1620,7 +1628,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>129.5</v>
+        <v>133.5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2195,7 +2203,7 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2378,8 +2386,12 @@
       <c r="D9" s="11">
         <v>4</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="E9" s="11">
+        <v>4</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0</v>
+      </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
@@ -2404,7 +2416,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>102.19999999999999</v>
+        <v>106.19999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2978,8 +2990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3164,8 +3176,12 @@
       <c r="D9" s="11">
         <v>4</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="E9" s="11">
+        <v>4</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0</v>
+      </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
@@ -3190,7 +3206,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>132.75</v>
+        <v>136.75</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated "Logboek and Urenlijst"
</commit_message>
<xml_diff>
--- a/Documenten/Urenlijst.xlsx
+++ b/Documenten/Urenlijst.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -12,7 +12,7 @@
     <sheet name="Remco" sheetId="2" r:id="rId3"/>
     <sheet name="Max" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -384,23 +384,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -436,23 +419,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -608,7 +574,7 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,7 +774,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="11">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="F9" s="11">
         <v>0</v>
@@ -837,7 +803,7 @@
       <c r="C11" s="20"/>
       <c r="D11" s="13">
         <f>SUM((C3,C4,C5,C6,C7,C8,C9,C10,D3,D4,D5,D6,D7,D8,D9,D10,E3,E4,E5,E6,E7,E8,E9,E10,F3,F4,F5,F6,F7,F8,F9,F10,G3,G4,G5,G6,G7,G8,G9,G10,H3,H4,H5,H6,H7,H8,H9,H10,I3,I4,I5,I6,I7,I8,I9,I10))</f>
-        <v>123.5</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>